<commit_message>
ARL tool, GUI and Paper 2 optimization complete TODO: Paper 1 optimization
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,51 +5,52 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="959" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gamma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTTRi</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Mb</t>
+  </si>
+  <si>
+    <t>c0</t>
+  </si>
+  <si>
+    <t>mub</t>
+  </si>
+  <si>
+    <t>mud</t>
+  </si>
+  <si>
+    <t>MTTRi</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>BA</t>
   </si>
 </sst>
 </file>
@@ -57,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -147,18 +148,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:J13"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -189,389 +190,467 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>20000</v>
+        <v>200000</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>200000</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1000000</v>
+        <v>5000000</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>5000000</v>
+        <v>0.9</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.9</v>
+        <v>24</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20000000</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>20000</v>
+        <v>75000</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>75000</v>
+        <v>500</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>200</v>
+        <v>8000000</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>8000000</v>
+        <v>4000000</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>4000000</v>
+        <v>0.8</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.8</v>
+        <v>36</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20000000</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>20000</v>
+        <v>90000</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>90000</v>
+        <v>700</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>400</v>
+        <v>6000000</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>6000000</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>6000000</v>
+        <v>0.85</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.85</v>
+        <v>40</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20000000</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>300</v>
+        <v>4000000</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>3000000</v>
+        <v>0.95</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.95</v>
+        <v>45</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>45</v>
+        <v>20000000</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>20000</v>
+        <v>200000</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>200000</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1000000</v>
+        <v>5000000</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>5000000</v>
+        <v>0.9</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.9</v>
+        <v>24</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>24</v>
+        <v>20000000</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>20000</v>
+        <v>75000</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>75000</v>
+        <v>500</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>200</v>
+        <v>8000000</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>8000000</v>
+        <v>4000000</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>4000000</v>
+        <v>0.8</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.8</v>
+        <v>36</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>36</v>
+        <v>20000000</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>20000</v>
+        <v>90000</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>90000</v>
+        <v>700</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>400</v>
+        <v>6000000</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>6000000</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>6000000</v>
+        <v>0.85</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.85</v>
+        <v>40</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>40</v>
+        <v>20000000</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>300</v>
+        <v>4000000</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>3000000</v>
+        <v>0.95</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.95</v>
+        <v>45</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>45</v>
+        <v>20000000</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>20000</v>
+        <v>200000</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>200000</v>
+        <v>1000</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1000000</v>
+        <v>5000000</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>5000000</v>
+        <v>0.9</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.9</v>
+        <v>24</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>24</v>
+        <v>20000000</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>20000</v>
+        <v>75000</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>75000</v>
+        <v>500</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>200</v>
+        <v>8000000</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>8000000</v>
+        <v>4000000</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>4000000</v>
+        <v>0.8</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.8</v>
+        <v>36</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>36</v>
+        <v>20000000</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>20000</v>
+        <v>90000</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>90000</v>
+        <v>700</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>400</v>
+        <v>6000000</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>6000000</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>6000000</v>
+        <v>0.85</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.85</v>
+        <v>40</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>40</v>
+        <v>20000000</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>300</v>
+        <v>4000000</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>3000000</v>
+        <v>0.95</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.95</v>
+        <v>45</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>1</v>
+        <v>20000</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>20000000</v>
+        <v>1</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>45</v>
+        <v>20000000</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>